<commit_message>
feat: connecting to mysql server
</commit_message>
<xml_diff>
--- a/BugTracker.xlsx
+++ b/BugTracker.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>No.</t>
   </si>
@@ -39,7 +39,19 @@
     <t>Status</t>
   </si>
   <si>
+    <t xml:space="preserve">authentication issue while connecting to mysql database</t>
+  </si>
+  <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>25/08/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Aldis</t>
+  </si>
+  <si>
+    <t>resolved</t>
   </si>
   <si>
     <t>Medium</t>
@@ -108,13 +120,17 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -630,13 +646,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="22.421875"/>
-    <col customWidth="1" min="4" max="4" width="9.8515625"/>
-    <col customWidth="1" min="5" max="5" style="1" width="13.57421875"/>
-    <col customWidth="1" min="6" max="6" width="18.00390625"/>
-    <col customWidth="1" min="7" max="7" width="16.421875"/>
-    <col customWidth="1" min="8" max="8" width="14.7109375"/>
-    <col customWidth="1" min="9" max="9" width="11.140625"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" width="22.421875"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="9.8515625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="13.57421875"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" width="18.00390625"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="16.421875"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" width="14.7109375"/>
+    <col bestFit="1" customWidth="1" min="9" max="9" width="11.140625"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.25">
@@ -665,25 +681,39 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="14.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+    <row r="3" ht="42.75">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -691,11 +721,11 @@
     </row>
     <row r="5" ht="14.25">
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="E5" s="6"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -703,9 +733,9 @@
     </row>
     <row r="6" ht="14.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -713,9 +743,9 @@
     </row>
     <row r="7" ht="14.25">
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -723,9 +753,9 @@
     </row>
     <row r="8" ht="14.25">
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -733,9 +763,9 @@
     </row>
     <row r="9" ht="14.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -743,9 +773,9 @@
     </row>
     <row r="10" ht="14.25">
       <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -753,9 +783,9 @@
     </row>
     <row r="11" ht="14.25">
       <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -763,9 +793,9 @@
     </row>
     <row r="12" ht="14.25">
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="C12" s="5"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -773,9 +803,9 @@
     </row>
     <row r="13" ht="14.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -783,9 +813,9 @@
     </row>
     <row r="14" ht="14.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -793,9 +823,9 @@
     </row>
     <row r="15" ht="14.25">
       <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="5"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -803,9 +833,9 @@
     </row>
     <row r="16" ht="14.25">
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -815,7 +845,7 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>

</xml_diff>